<commit_message>
Update Competitions before Quarterfinals
</commit_message>
<xml_diff>
--- a/2023WinLose.xlsx
+++ b/2023WinLose.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xilin\Documents\Application\final project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBF7D88-5BAE-41EA-B33A-8151A837B80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FC671A-5D43-458A-BFA3-A3FD3D312259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13630" yWindow="3520" windowWidth="15880" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="19">
   <si>
     <t>Team1</t>
   </si>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -751,6 +751,248 @@
         <v>0</v>
       </c>
     </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>